<commit_message>
client requests added; enhanced ui
</commit_message>
<xml_diff>
--- a/public/download/MultiIndividualFormat.xlsx
+++ b/public/download/MultiIndividualFormat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kms\public\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RJ Marcial\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40174577-0108-42AB-B427-2B46A4872C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E948F2F-E95D-49D4-A392-0ED2A4246F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{607CB8D3-4C4C-4EEC-9EC1-C30247810F06}"/>
   </bookViews>
@@ -36,27 +36,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Middle Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Birthdate (YYYY-MM-DD)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Height (cm)</t>
   </si>
   <si>
-    <t>Weight (kg)</t>
+    <t>Last Name of Child</t>
+  </si>
+  <si>
+    <t>First Name of Child</t>
+  </si>
+  <si>
+    <t>Address or Location
+of Child's Residence</t>
+  </si>
+  <si>
+    <t>Birthdate
+(YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Weight (cm)</t>
+  </si>
+  <si>
+    <t>Belongs to IP Group?
+(Yes/No)</t>
+  </si>
+  <si>
+    <t>Sex
+(Male/Female)</t>
+  </si>
+  <si>
+    <t>Taking Micronutrient Supplementation?
+(Yes/No)</t>
+  </si>
+  <si>
+    <t>Last Name
+of Parent/Guardian</t>
+  </si>
+  <si>
+    <t>First Name
+of Parent/Guardian</t>
   </si>
 </sst>
 </file>
@@ -106,11 +125,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,53 +448,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481E7E0C-D94B-4034-9D47-B91F995936A1}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="7" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
     </row>
   </sheetData>

</xml_diff>